<commit_message>
updated required changes, pr lines, new liquidation features
</commit_message>
<xml_diff>
--- a/Full_Report.xlsx
+++ b/Full_Report.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="88">
   <si>
     <t>id</t>
   </si>
@@ -92,22 +92,13 @@
     <t>assigned_to</t>
   </si>
   <si>
-    <t>project_code</t>
-  </si>
-  <si>
-    <t>task_number</t>
-  </si>
-  <si>
-    <t>task_desc</t>
-  </si>
-  <si>
-    <t>wbl_percentage</t>
-  </si>
-  <si>
-    <t>pr123</t>
-  </si>
-  <si>
-    <t>2025-09-23</t>
+    <t>p0123</t>
+  </si>
+  <si>
+    <t>pr12323</t>
+  </si>
+  <si>
+    <t>2025-10-02</t>
   </si>
   <si>
     <t>admin</t>
@@ -116,40 +107,46 @@
     <t>CRLR</t>
   </si>
   <si>
-    <t>Services</t>
+    <t>Goods</t>
   </si>
   <si>
     <t>Rental Vehicle</t>
   </si>
   <si>
+    <t>ssss</t>
+  </si>
+  <si>
     <t>Sedan Car</t>
   </si>
   <si>
     <t>fahad</t>
   </si>
   <si>
-    <t>03445471211</t>
-  </si>
-  <si>
-    <t>2025-09-25</t>
+    <t>11111111111</t>
+  </si>
+  <si>
+    <t>1111111</t>
+  </si>
+  <si>
+    <t>2025-10-01</t>
   </si>
   <si>
     <t>Islamabad</t>
   </si>
   <si>
-    <t>karachi</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>Submitted</t>
   </si>
   <si>
-    <t>2025-09-23 09:53:02.283756</t>
-  </si>
-  <si>
-    <t>2025-09-23 09:53:29.415544</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>2025-10-02 15:54:37.236771</t>
+  </si>
+  <si>
+    <t>2025-10-02 16:04:51.683825</t>
   </si>
   <si>
     <t>pr_id</t>
@@ -164,6 +161,9 @@
     <t>wave_receipt</t>
   </si>
   <si>
+    <t>work_confirmation</t>
+  </si>
+  <si>
     <t>work_order_yesno</t>
   </si>
   <si>
@@ -182,6 +182,27 @@
     <t>remarks</t>
   </si>
   <si>
+    <t>po123</t>
+  </si>
+  <si>
+    <t>p333</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>dad</t>
+  </si>
+  <si>
+    <t>In Process</t>
+  </si>
+  <si>
+    <t>2025-10-02 10:57:17</t>
+  </si>
+  <si>
+    <t>2025-10-02 11:06:33</t>
+  </si>
+  <si>
     <t>dsa_type</t>
   </si>
   <si>
@@ -239,10 +260,28 @@
     <t>PR</t>
   </si>
   <si>
-    <t>2025-09-23 04:53:02</t>
-  </si>
-  <si>
-    <t>2025-09-23 04:53:29</t>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>2025-10-02 10:54:37</t>
+  </si>
+  <si>
+    <t>2025-10-02 10:57:47</t>
+  </si>
+  <si>
+    <t>2025-10-02 11:04:51</t>
+  </si>
+  <si>
+    <t>2025-10-02 11:07:12</t>
   </si>
 </sst>
 </file>
@@ -600,13 +639,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,153 +718,144 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>36</v>
       </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
       <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
         <v>37</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>2</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
         <v>38</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2" t="s">
-        <v>40</v>
       </c>
       <c r="T2">
         <v>1</v>
       </c>
       <c r="V2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" t="s">
         <v>41</v>
       </c>
-      <c r="W2" t="s">
-        <v>42</v>
-      </c>
       <c r="X2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>33</v>
       </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>36</v>
       </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
       <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
         <v>37</v>
-      </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-      <c r="O3" t="s">
-        <v>39</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="R3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="S3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
       <c r="V3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -835,54 +865,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -915,10 +1033,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -927,19 +1045,19 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>20</v>
@@ -978,25 +1096,25 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>14</v>
@@ -1018,7 +1136,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1029,22 +1147,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1052,19 +1170,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1072,19 +1190,128 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>